<commit_message>
File Sending Write Posing Or insart e-bill 70
</commit_message>
<xml_diff>
--- a/E-Bill (2).xlsx
+++ b/E-Bill (2).xlsx
@@ -1158,6 +1158,66 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1179,67 +1239,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1282,24 +1300,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1660,7 +1660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1723,10 +1723,10 @@
       <c r="I2" s="77"/>
       <c r="J2" s="77"/>
       <c r="K2" s="77"/>
-      <c r="L2" s="175" t="s">
+      <c r="L2" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="176"/>
+      <c r="M2" s="165"/>
     </row>
     <row r="3" spans="2:20" ht="23.25" customHeight="1">
       <c r="B3" s="93"/>
@@ -1780,11 +1780,11 @@
       <c r="H5" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="172" t="s">
+      <c r="I5" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
       <c r="L5" s="33"/>
       <c r="M5" s="97"/>
     </row>
@@ -1798,11 +1798,11 @@
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
-      <c r="I6" s="172" t="s">
+      <c r="I6" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="172"/>
-      <c r="K6" s="172"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="178"/>
       <c r="L6" s="33"/>
       <c r="M6" s="97"/>
       <c r="P6" s="98">
@@ -1810,18 +1810,18 @@
       </c>
     </row>
     <row r="7" spans="2:20">
-      <c r="B7" s="187" t="s">
+      <c r="B7" s="176" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
-      <c r="I7" s="172"/>
-      <c r="J7" s="172"/>
-      <c r="K7" s="172"/>
+      <c r="I7" s="178"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="178"/>
       <c r="L7" s="33"/>
       <c r="M7" s="97"/>
     </row>
@@ -1835,11 +1835,11 @@
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
-      <c r="I8" s="188" t="s">
+      <c r="I8" s="179" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="188"/>
-      <c r="K8" s="188"/>
+      <c r="J8" s="179"/>
+      <c r="K8" s="179"/>
       <c r="L8" s="33"/>
       <c r="M8" s="97"/>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="C9" s="100">
         <f ca="1">TODAY()</f>
-        <v>44241</v>
+        <v>44245</v>
       </c>
       <c r="D9" s="101"/>
       <c r="E9" s="101"/>
@@ -1858,10 +1858,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="101"/>
-      <c r="I9" s="167" t="s">
+      <c r="I9" s="187" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="168"/>
+      <c r="J9" s="188"/>
       <c r="K9" s="101" t="s">
         <v>2</v>
       </c>
@@ -1875,24 +1875,24 @@
       </c>
     </row>
     <row r="10" spans="2:20" ht="16.5" thickBot="1">
-      <c r="B10" s="189" t="s">
+      <c r="B10" s="180" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
+      <c r="C10" s="181"/>
+      <c r="D10" s="181"/>
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
-      <c r="I10" s="169"/>
-      <c r="J10" s="170"/>
+      <c r="I10" s="189"/>
+      <c r="J10" s="190"/>
       <c r="K10" s="33" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="33"/>
       <c r="M10" s="103">
         <f ca="1">TODAY()</f>
-        <v>44241</v>
+        <v>44245</v>
       </c>
       <c r="R10" s="104" t="s">
         <v>10</v>
@@ -2541,10 +2541,10 @@
       </c>
       <c r="O31" s="128"/>
       <c r="P31" s="98"/>
-      <c r="Q31" s="166" t="s">
+      <c r="Q31" s="186" t="s">
         <v>37</v>
       </c>
-      <c r="R31" s="166"/>
+      <c r="R31" s="186"/>
       <c r="S31" s="91" t="e">
         <f>T29-R29</f>
         <v>#REF!</v>
@@ -2618,15 +2618,15 @@
       <c r="S34" s="98"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="B35" s="191" t="s">
+      <c r="B35" s="182" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="192"/>
-      <c r="D35" s="192"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
+      <c r="C35" s="183"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="183"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
       <c r="I35" s="137"/>
       <c r="J35" s="137"/>
       <c r="K35" s="137"/>
@@ -2634,37 +2634,37 @@
       <c r="M35" s="138"/>
     </row>
     <row r="36" spans="1:19">
-      <c r="B36" s="183"/>
-      <c r="C36" s="178"/>
-      <c r="D36" s="178"/>
-      <c r="E36" s="184"/>
+      <c r="B36" s="172"/>
+      <c r="C36" s="167"/>
+      <c r="D36" s="167"/>
+      <c r="E36" s="173"/>
       <c r="F36" s="139"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
       <c r="J36" s="33"/>
-      <c r="K36" s="177" t="s">
+      <c r="K36" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="L36" s="178"/>
-      <c r="M36" s="179"/>
+      <c r="L36" s="167"/>
+      <c r="M36" s="168"/>
       <c r="P36" s="91" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B37" s="185"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="186"/>
+      <c r="B37" s="174"/>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="175"/>
       <c r="F37" s="140"/>
       <c r="G37" s="141"/>
       <c r="H37" s="141"/>
       <c r="I37" s="141"/>
       <c r="J37" s="141"/>
-      <c r="K37" s="180"/>
-      <c r="L37" s="181"/>
-      <c r="M37" s="182"/>
+      <c r="K37" s="169"/>
+      <c r="L37" s="170"/>
+      <c r="M37" s="171"/>
       <c r="S37" s="91" t="e">
         <f>SUM(S24:S36)</f>
         <v>#REF!</v>
@@ -2712,8 +2712,8 @@
       <c r="I40" s="33"/>
       <c r="J40" s="33"/>
       <c r="K40" s="33"/>
-      <c r="L40" s="171"/>
-      <c r="M40" s="171"/>
+      <c r="L40" s="177"/>
+      <c r="M40" s="177"/>
     </row>
     <row r="41" spans="1:19" ht="17.25">
       <c r="A41" s="33"/>
@@ -2754,9 +2754,9 @@
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="172"/>
-      <c r="J43" s="172"/>
-      <c r="K43" s="172"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="178"/>
+      <c r="K43" s="178"/>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
     </row>
@@ -2769,24 +2769,24 @@
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
       <c r="H44" s="33"/>
-      <c r="I44" s="172"/>
-      <c r="J44" s="172"/>
-      <c r="K44" s="172"/>
+      <c r="I44" s="178"/>
+      <c r="J44" s="178"/>
+      <c r="K44" s="178"/>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="33"/>
-      <c r="B45" s="171"/>
-      <c r="C45" s="171"/>
-      <c r="D45" s="171"/>
-      <c r="E45" s="171"/>
+      <c r="B45" s="177"/>
+      <c r="C45" s="177"/>
+      <c r="D45" s="177"/>
+      <c r="E45" s="177"/>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
-      <c r="I45" s="172"/>
-      <c r="J45" s="172"/>
-      <c r="K45" s="172"/>
+      <c r="I45" s="178"/>
+      <c r="J45" s="178"/>
+      <c r="K45" s="178"/>
       <c r="L45" s="33"/>
       <c r="M45" s="33"/>
     </row>
@@ -2799,9 +2799,9 @@
       <c r="F46" s="36"/>
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
-      <c r="I46" s="173"/>
-      <c r="J46" s="173"/>
-      <c r="K46" s="173"/>
+      <c r="I46" s="191"/>
+      <c r="J46" s="191"/>
+      <c r="K46" s="191"/>
       <c r="L46" s="36"/>
       <c r="M46" s="36"/>
       <c r="N46" s="36"/>
@@ -2819,8 +2819,8 @@
       <c r="J47" s="36"/>
       <c r="K47" s="36"/>
       <c r="L47" s="36"/>
-      <c r="M47" s="173"/>
-      <c r="N47" s="173"/>
+      <c r="M47" s="191"/>
+      <c r="N47" s="191"/>
       <c r="O47" s="33"/>
     </row>
     <row r="48" spans="1:19" ht="15" customHeight="1">
@@ -2909,10 +2909,10 @@
     </row>
     <row r="52" spans="2:15">
       <c r="B52" s="36"/>
-      <c r="C52" s="173"/>
-      <c r="D52" s="173"/>
-      <c r="E52" s="173"/>
-      <c r="F52" s="173"/>
+      <c r="C52" s="191"/>
+      <c r="D52" s="191"/>
+      <c r="E52" s="191"/>
+      <c r="F52" s="191"/>
       <c r="G52" s="36"/>
       <c r="H52" s="149" t="s">
         <v>54</v>
@@ -2987,9 +2987,9 @@
     </row>
     <row r="55" spans="2:15">
       <c r="B55" s="36"/>
-      <c r="C55" s="174"/>
-      <c r="D55" s="174"/>
-      <c r="E55" s="174"/>
+      <c r="C55" s="192"/>
+      <c r="D55" s="192"/>
+      <c r="E55" s="192"/>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="37" t="s">
@@ -3545,13 +3545,13 @@
     </row>
     <row r="78" spans="2:15">
       <c r="B78" s="36"/>
-      <c r="C78" s="164"/>
-      <c r="D78" s="164"/>
-      <c r="E78" s="164"/>
-      <c r="F78" s="164"/>
-      <c r="G78" s="164"/>
-      <c r="H78" s="164"/>
-      <c r="I78" s="164"/>
+      <c r="C78" s="184"/>
+      <c r="D78" s="184"/>
+      <c r="E78" s="184"/>
+      <c r="F78" s="184"/>
+      <c r="G78" s="184"/>
+      <c r="H78" s="184"/>
+      <c r="I78" s="184"/>
       <c r="J78" s="36"/>
       <c r="K78" s="36"/>
       <c r="L78" s="36"/>
@@ -3561,34 +3561,34 @@
     </row>
     <row r="79" spans="2:15">
       <c r="B79" s="36"/>
-      <c r="C79" s="165"/>
-      <c r="D79" s="165"/>
-      <c r="E79" s="165"/>
-      <c r="F79" s="165"/>
+      <c r="C79" s="185"/>
+      <c r="D79" s="185"/>
+      <c r="E79" s="185"/>
+      <c r="F79" s="185"/>
       <c r="G79" s="156"/>
       <c r="H79" s="36"/>
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
       <c r="K79" s="36"/>
-      <c r="L79" s="165"/>
-      <c r="M79" s="165"/>
-      <c r="N79" s="165"/>
+      <c r="L79" s="185"/>
+      <c r="M79" s="185"/>
+      <c r="N79" s="185"/>
       <c r="O79" s="33"/>
     </row>
     <row r="80" spans="2:15">
       <c r="B80" s="36"/>
-      <c r="C80" s="165"/>
-      <c r="D80" s="165"/>
-      <c r="E80" s="165"/>
-      <c r="F80" s="165"/>
+      <c r="C80" s="185"/>
+      <c r="D80" s="185"/>
+      <c r="E80" s="185"/>
+      <c r="F80" s="185"/>
       <c r="G80" s="156"/>
       <c r="H80" s="36"/>
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>
       <c r="K80" s="36"/>
-      <c r="L80" s="165"/>
-      <c r="M80" s="165"/>
-      <c r="N80" s="165"/>
+      <c r="L80" s="185"/>
+      <c r="M80" s="185"/>
+      <c r="N80" s="185"/>
       <c r="O80" s="33"/>
     </row>
     <row r="81" spans="2:15">
@@ -3641,16 +3641,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="K36:M37"/>
-    <mergeCell ref="B36:E37"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B35:H35"/>
     <mergeCell ref="C78:I78"/>
     <mergeCell ref="C79:F80"/>
     <mergeCell ref="L79:N80"/>
@@ -3665,6 +3655,16 @@
     <mergeCell ref="M47:N47"/>
     <mergeCell ref="C52:F52"/>
     <mergeCell ref="C55:E55"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="K36:M37"/>
+    <mergeCell ref="B36:E37"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B35:H35"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.24803149599999999" bottom="0.25" header="0.31496062992126" footer="0.31496062992126"/>
@@ -3700,8 +3700,8 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="208"/>
-      <c r="M3" s="209"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="195"/>
     </row>
     <row r="4" spans="2:13" ht="28.5">
       <c r="B4" s="8"/>
@@ -3739,9 +3739,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="210"/>
-      <c r="J6" s="210"/>
-      <c r="K6" s="210"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="196"/>
+      <c r="K6" s="196"/>
       <c r="L6" s="1"/>
       <c r="M6" s="9"/>
     </row>
@@ -3753,23 +3753,23 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="210"/>
-      <c r="J7" s="210"/>
-      <c r="K7" s="210"/>
+      <c r="I7" s="196"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
       <c r="L7" s="1"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="211"/>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
+      <c r="B8" s="197"/>
+      <c r="C8" s="198"/>
+      <c r="D8" s="198"/>
+      <c r="E8" s="198"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="210"/>
-      <c r="J8" s="210"/>
-      <c r="K8" s="210"/>
+      <c r="I8" s="196"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="196"/>
       <c r="L8" s="1"/>
       <c r="M8" s="9"/>
     </row>
@@ -3781,9 +3781,9 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="207"/>
-      <c r="J9" s="207"/>
-      <c r="K9" s="207"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="193"/>
       <c r="L9" s="1"/>
       <c r="M9" s="9"/>
     </row>
@@ -3795,22 +3795,22 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="167"/>
-      <c r="J10" s="168"/>
+      <c r="I10" s="187"/>
+      <c r="J10" s="188"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B11" s="193"/>
-      <c r="C11" s="194"/>
-      <c r="D11" s="194"/>
+      <c r="B11" s="199"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="200"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="170"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="190"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="63"/>
@@ -4208,13 +4208,13 @@
       <c r="M39" s="30"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="195"/>
-      <c r="C40" s="196"/>
-      <c r="D40" s="196"/>
-      <c r="E40" s="196"/>
-      <c r="F40" s="196"/>
-      <c r="G40" s="196"/>
-      <c r="H40" s="196"/>
+      <c r="B40" s="201"/>
+      <c r="C40" s="202"/>
+      <c r="D40" s="202"/>
+      <c r="E40" s="202"/>
+      <c r="F40" s="202"/>
+      <c r="G40" s="202"/>
+      <c r="H40" s="202"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -4222,46 +4222,46 @@
       <c r="M40" s="12"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="197"/>
-      <c r="C41" s="198"/>
-      <c r="D41" s="198"/>
-      <c r="E41" s="199"/>
+      <c r="B41" s="203"/>
+      <c r="C41" s="204"/>
+      <c r="D41" s="204"/>
+      <c r="E41" s="205"/>
       <c r="F41" s="23"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="203"/>
-      <c r="L41" s="198"/>
-      <c r="M41" s="204"/>
+      <c r="K41" s="209"/>
+      <c r="L41" s="204"/>
+      <c r="M41" s="210"/>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B42" s="200"/>
-      <c r="C42" s="201"/>
-      <c r="D42" s="201"/>
-      <c r="E42" s="202"/>
+      <c r="B42" s="206"/>
+      <c r="C42" s="207"/>
+      <c r="D42" s="207"/>
+      <c r="E42" s="208"/>
       <c r="F42" s="57"/>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
-      <c r="K42" s="205"/>
-      <c r="L42" s="201"/>
-      <c r="M42" s="206"/>
+      <c r="K42" s="211"/>
+      <c r="L42" s="207"/>
+      <c r="M42" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:E42"/>
+    <mergeCell ref="K41:M42"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:E42"/>
-    <mergeCell ref="K41:M42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
job work 12 pm 11/03/2021
</commit_message>
<xml_diff>
--- a/E-Bill (2).xlsx
+++ b/E-Bill (2).xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="880" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$13:$H$24</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$M$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$H$13:$H$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$2:$M$37</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>DATE :</t>
   </si>
@@ -134,18 +135,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>You have Save  =</t>
-  </si>
-  <si>
     <t>Sugar</t>
   </si>
   <si>
-    <t>pkt.</t>
-  </si>
-  <si>
     <t>Maida</t>
   </si>
   <si>
@@ -215,49 +207,43 @@
     <t xml:space="preserve"> Vim Lemon Soap (155gm)</t>
   </si>
   <si>
-    <t>Tata Salt (500 gm.)</t>
-  </si>
-  <si>
-    <t>Sunrise Termaric Powder (50 gm.)</t>
-  </si>
-  <si>
-    <t>Sunrise Jeera Powder (50 gm.)</t>
-  </si>
-  <si>
-    <t>Sunrise Dhiniya Podwer (50 gm.)</t>
-  </si>
-  <si>
-    <t>Kamal Moosoor Dal (500 gm.)</t>
-  </si>
-  <si>
     <t>gm.</t>
   </si>
   <si>
-    <t>pc.</t>
-  </si>
-  <si>
-    <t>Shalimar Coconut Oil (175 ml)</t>
-  </si>
-  <si>
-    <t>Britannia Nutri choice thin Arrowroot (300 gm.)</t>
-  </si>
-  <si>
-    <t>Colgate Strong Teeth ( 200 gm.)</t>
-  </si>
-  <si>
-    <t>Ms. Supriya</t>
-  </si>
-  <si>
-    <t>Four Hundred Four Rupees Only</t>
-  </si>
-  <si>
-    <t>Bill No-75</t>
-  </si>
-  <si>
-    <t>Nischintopur</t>
-  </si>
-  <si>
-    <t>PHONE NO-9830853299</t>
+    <t>kg.</t>
+  </si>
+  <si>
+    <t>Bill No-78</t>
+  </si>
+  <si>
+    <t>Emami Kachhi Ghani Pouch ( 1 lt.)</t>
+  </si>
+  <si>
+    <t>lt.</t>
+  </si>
+  <si>
+    <t>Emami Healthy Testy soyabean oil(1 lt)</t>
+  </si>
+  <si>
+    <t>Kamal Moosoor Dal</t>
+  </si>
+  <si>
+    <t>Mayda</t>
+  </si>
+  <si>
+    <t>Moog Dal</t>
+  </si>
+  <si>
+    <t>Mr.  Anupkumar Nath</t>
+  </si>
+  <si>
+    <t>PHONE NO-9903058205</t>
+  </si>
+  <si>
+    <t>Pujali Pal Para</t>
+  </si>
+  <si>
+    <t>Five Hundred Forty Four  Rupees Only</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1052,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1130,7 +1115,6 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1151,25 +1135,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1331,7 +1321,532 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bill No-78 Page :</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$9:$K$24</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Invoice No.      :</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Invoice Date    :</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>RATE</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v> 145.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v> 132.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v> 42.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v> 100.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> 25.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v> 130.00 </c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v> INVOICE</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>MRP</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v> 180.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v> 160.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v> 43.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v> 110.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>27.00</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v> 140.00 </c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Product Description</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Emami Kachhi Ghani Pouch ( 1 lt.)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Emami Healthy Testy soyabean oil(1 lt)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sugar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Kamal Moosoor Dal</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Mayda</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Moog Dal</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SLOT :</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Pack</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Exp. Date</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Free</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>U.O.M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>lt.</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>lt.</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>gm.</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3/2/2021</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qty.</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>250</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>DATE :</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CARRET NO : Gro On</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sl No.</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$9:$L$24</c:f>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bill No-78 01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$9:$K$24</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Invoice No.      :</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Invoice Date    :</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>RATE</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v> 145.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v> 132.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v> 42.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v> 100.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v> 25.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v> 130.00 </c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v> INVOICE</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>MRP</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v> 180.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v> 160.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v> 43.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v> 110.00 </c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>27.00</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v> 140.00 </c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Product Description</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Emami Kachhi Ghani Pouch ( 1 lt.)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Emami Healthy Testy soyabean oil(1 lt)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sugar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Kamal Moosoor Dal</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Mayda</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Moog Dal</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SLOT :</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Pack</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Exp. Date</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Free</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>U.O.M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>lt.</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>lt.</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>kg.</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>gm.</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3/2/2021</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qty.</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>250</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>DATE :</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CARRET NO : Gro On</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sl No.</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$9:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44257</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>32.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="54690944"/>
+        <c:axId val="54692480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="54690944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54692480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54692480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54690944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1374,7 +1889,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1683,7 +2198,7 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="63" zoomScaleNormal="63" zoomScaleSheetLayoutView="56" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1736,7 +2251,7 @@
       <c r="J2" s="77"/>
       <c r="K2" s="77"/>
       <c r="L2" s="168" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="M2" s="169"/>
     </row>
@@ -1777,7 +2292,7 @@
       <c r="M4" s="97"/>
       <c r="P4" s="98">
         <f>SUM(J12:J18)</f>
-        <v>264</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="2:20">
@@ -1789,9 +2304,9 @@
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
-      <c r="H5" s="128"/>
+      <c r="H5" s="127"/>
       <c r="I5" s="182" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J5" s="182"/>
       <c r="K5" s="182"/>
@@ -1809,7 +2324,7 @@
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
       <c r="I6" s="182" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J6" s="182"/>
       <c r="K6" s="182"/>
@@ -1846,7 +2361,7 @@
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
       <c r="I8" s="183" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J8" s="183"/>
       <c r="K8" s="183"/>
@@ -1859,7 +2374,7 @@
       </c>
       <c r="C9" s="100">
         <f ca="1">TODAY()</f>
-        <v>44253</v>
+        <v>44257</v>
       </c>
       <c r="D9" s="101"/>
       <c r="E9" s="101"/>
@@ -1877,11 +2392,11 @@
       </c>
       <c r="L9" s="101"/>
       <c r="M9" s="102">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="R9" s="98">
         <f>SUM(O12:O27)</f>
-        <v>1329</v>
+        <v>1793.5</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="16.5" thickBot="1">
@@ -1902,7 +2417,7 @@
       <c r="L10" s="33"/>
       <c r="M10" s="103">
         <f ca="1">TODAY()</f>
-        <v>44253</v>
+        <v>44257</v>
       </c>
       <c r="R10" s="104" t="s">
         <v>10</v>
@@ -1946,37 +2461,36 @@
       </c>
     </row>
     <row r="12" spans="2:20">
-      <c r="B12" s="112">
+      <c r="B12" s="165">
         <v>1</v>
       </c>
-      <c r="C12" s="158">
-        <v>4</v>
+      <c r="C12" s="156">
+        <v>1</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E12" s="76"/>
       <c r="F12" s="77"/>
       <c r="G12" s="76"/>
-      <c r="H12" s="167" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="166">
-        <v>14</v>
+      <c r="H12" s="162" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="163">
+        <v>180</v>
       </c>
       <c r="J12" s="49">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="K12" s="77"/>
       <c r="L12" s="77"/>
       <c r="M12" s="79">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="O12" s="98">
-        <f>14*4</f>
-        <v>56</v>
-      </c>
-      <c r="P12" s="113"/>
+        <v>180</v>
+      </c>
+      <c r="P12" s="112"/>
       <c r="Q12" s="98"/>
       <c r="R12" s="91" t="e">
         <f>IF(#REF!="lt.",D57*J57,IF(#REF!="gm.",D57/1000*J57,IF(#REF!="pkt.",D57*J57,IF(#REF!="kg.",D57*J57,IF(#REF!="ml.",D57/1000*RJ1501)))))</f>
@@ -1988,36 +2502,36 @@
       </c>
     </row>
     <row r="13" spans="2:20">
-      <c r="B13" s="114">
+      <c r="B13" s="166">
         <v>2</v>
       </c>
-      <c r="C13" s="159">
-        <v>2</v>
+      <c r="C13" s="157">
+        <v>1</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="156"/>
-      <c r="H13" s="157" t="s">
+      <c r="G13" s="154"/>
+      <c r="H13" s="155" t="s">
         <v>65</v>
       </c>
       <c r="I13" s="161">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="J13" s="50">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="K13" s="33"/>
       <c r="L13" s="33"/>
       <c r="M13" s="31">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="O13" s="98">
-        <v>50</v>
-      </c>
-      <c r="P13" s="113"/>
+        <v>160</v>
+      </c>
+      <c r="P13" s="112"/>
       <c r="R13" s="91" t="b">
         <f>IF(D58="lt.",C58*J58,IF(D58="gm.",C58/1000*J58,IF(D58="pkt.",C58*J58,IF(D58="kg.",C58*J58,IF(D58="ml.",C58/1000*RJ1502)))))</f>
         <v>0</v>
@@ -2028,52 +2542,52 @@
       </c>
     </row>
     <row r="14" spans="2:20">
-      <c r="B14" s="114">
+      <c r="B14" s="166">
         <v>3</v>
       </c>
-      <c r="C14" s="159">
+      <c r="C14" s="157">
         <v>2</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
-      <c r="G14" s="156"/>
-      <c r="H14" s="157" t="s">
-        <v>66</v>
+      <c r="G14" s="154"/>
+      <c r="H14" s="155" t="s">
+        <v>36</v>
       </c>
       <c r="I14" s="161">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="J14" s="50">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="K14" s="33"/>
       <c r="L14" s="33"/>
       <c r="M14" s="31">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="O14" s="98">
-        <v>32</v>
-      </c>
-      <c r="P14" s="113"/>
+        <v>86</v>
+      </c>
+      <c r="P14" s="112"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="B15" s="114">
+      <c r="B15" s="166">
         <v>4</v>
       </c>
-      <c r="C15" s="159">
-        <v>500</v>
+      <c r="C15" s="157">
+        <v>1</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="164"/>
+        <v>61</v>
+      </c>
+      <c r="E15" s="160"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="156"/>
+      <c r="G15" s="154"/>
       <c r="H15" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I15" s="161">
         <v>110</v>
@@ -2084,12 +2598,12 @@
       <c r="K15" s="33"/>
       <c r="L15" s="33"/>
       <c r="M15" s="31">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O15" s="98">
-        <v>55</v>
-      </c>
-      <c r="P15" s="113"/>
+        <v>110</v>
+      </c>
+      <c r="P15" s="112"/>
       <c r="R15" s="91" t="b">
         <f t="shared" ref="R15:R24" si="0">IF(D59="lt.",C59*J59,IF(D59="gm.",C59/1000*J59,IF(D59="pkt.",C59*J59,IF(D59="kg.",C59*J59,IF(D59="ml.",C59/1000*RJ1503)))))</f>
         <v>0</v>
@@ -2100,36 +2614,36 @@
       </c>
     </row>
     <row r="16" spans="2:20" ht="16.5" customHeight="1">
-      <c r="B16" s="114">
+      <c r="B16" s="166">
         <v>5</v>
       </c>
-      <c r="C16" s="159">
-        <v>4</v>
-      </c>
-      <c r="D16" s="160" t="s">
-        <v>39</v>
+      <c r="C16" s="157">
+        <v>2</v>
+      </c>
+      <c r="D16" s="158" t="s">
+        <v>61</v>
       </c>
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
-      <c r="H16" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="162">
-        <v>11</v>
+      <c r="H16" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="159">
+        <v>27</v>
       </c>
       <c r="J16" s="50">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
       <c r="M16" s="31">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="O16" s="98">
-        <v>44</v>
-      </c>
-      <c r="P16" s="113"/>
+        <v>54</v>
+      </c>
+      <c r="P16" s="112"/>
       <c r="R16" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2140,36 +2654,36 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="114">
+      <c r="B17" s="166">
         <v>6</v>
       </c>
-      <c r="C17" s="160">
-        <v>1</v>
+      <c r="C17" s="158">
+        <v>250</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E17" s="65"/>
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="157" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="163">
-        <v>76</v>
+      <c r="H17" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="164">
+        <v>140</v>
       </c>
       <c r="J17" s="66">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="K17" s="65"/>
       <c r="L17" s="33"/>
       <c r="M17" s="31">
-        <v>74</v>
+        <v>32.5</v>
       </c>
       <c r="O17" s="98">
-        <v>76</v>
-      </c>
-      <c r="P17" s="113"/>
+        <v>35</v>
+      </c>
+      <c r="P17" s="112"/>
       <c r="R17" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2180,37 +2694,21 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="114">
-        <v>7</v>
-      </c>
-      <c r="C18" s="160">
-        <v>1</v>
-      </c>
-      <c r="D18" s="43" t="s">
-        <v>39</v>
-      </c>
+      <c r="B18" s="166"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
-      <c r="H18" s="157" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" s="163">
-        <v>35</v>
-      </c>
-      <c r="J18" s="50">
-        <v>34</v>
-      </c>
+      <c r="H18" s="155"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="50"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
-      <c r="M18" s="31">
-        <v>34</v>
-      </c>
+      <c r="M18" s="31"/>
       <c r="N18" s="31"/>
-      <c r="O18" s="98">
-        <v>35</v>
-      </c>
-      <c r="P18" s="113"/>
+      <c r="O18" s="98"/>
+      <c r="P18" s="112"/>
       <c r="R18" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2221,37 +2719,21 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="114">
-        <v>8</v>
-      </c>
-      <c r="C19" s="160">
-        <v>1</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>39</v>
-      </c>
+      <c r="B19" s="166"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
       <c r="G19" s="33"/>
-      <c r="H19" s="157" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" s="163">
-        <v>95</v>
-      </c>
-      <c r="J19" s="50">
-        <v>94</v>
-      </c>
+      <c r="H19" s="155"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="50"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
-      <c r="M19" s="31">
-        <v>94</v>
-      </c>
+      <c r="M19" s="31"/>
       <c r="N19" s="58"/>
-      <c r="O19" s="98">
-        <v>95</v>
-      </c>
-      <c r="P19" s="113"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="112"/>
       <c r="R19" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2262,20 +2744,20 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="114"/>
-      <c r="C20" s="160"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="158"/>
       <c r="D20" s="43"/>
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
       <c r="G20" s="33"/>
-      <c r="H20" s="115"/>
+      <c r="H20" s="155"/>
       <c r="I20" s="161"/>
       <c r="J20" s="50"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
       <c r="M20" s="31"/>
       <c r="O20" s="98"/>
-      <c r="P20" s="113"/>
+      <c r="P20" s="112"/>
       <c r="R20" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2286,23 +2768,23 @@
       </c>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="114"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="158"/>
       <c r="D21" s="43"/>
       <c r="E21" s="33"/>
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="115"/>
-      <c r="I21" s="165"/>
+      <c r="H21" s="114"/>
+      <c r="I21" s="161"/>
       <c r="J21" s="50"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
       <c r="M21" s="31"/>
       <c r="O21" s="98">
-        <f>SUM(O12:O19)</f>
-        <v>443</v>
-      </c>
-      <c r="P21" s="113"/>
+        <f>SUM(O12:O17)</f>
+        <v>625</v>
+      </c>
+      <c r="P21" s="112"/>
       <c r="R21" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2313,20 +2795,20 @@
       </c>
     </row>
     <row r="22" spans="2:20">
-      <c r="B22" s="114"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="43"/>
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="165"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="161"/>
       <c r="J22" s="50"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
       <c r="M22" s="31"/>
       <c r="O22" s="98"/>
-      <c r="P22" s="113"/>
+      <c r="P22" s="112"/>
       <c r="R22" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2337,40 +2819,40 @@
       </c>
     </row>
     <row r="23" spans="2:20">
-      <c r="B23" s="114"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="158"/>
       <c r="D23" s="43"/>
       <c r="E23" s="33"/>
       <c r="F23" s="33"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="150"/>
-      <c r="I23" s="50"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="167"/>
       <c r="J23" s="50"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
       <c r="M23" s="31"/>
       <c r="O23" s="98"/>
-      <c r="P23" s="113"/>
+      <c r="P23" s="112"/>
       <c r="R23" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:20">
-      <c r="B24" s="114"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="158"/>
       <c r="D24" s="43"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="115"/>
-      <c r="I24" s="50"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="114"/>
+      <c r="I24" s="167"/>
       <c r="J24" s="50"/>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
       <c r="M24" s="31"/>
       <c r="O24" s="98"/>
-      <c r="P24" s="113"/>
+      <c r="P24" s="112"/>
       <c r="R24" s="91" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2381,39 +2863,39 @@
       </c>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="114"/>
+      <c r="B25" s="113"/>
       <c r="C25" s="40"/>
       <c r="D25" s="43"/>
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="50"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="114"/>
+      <c r="I25" s="167"/>
       <c r="J25" s="50"/>
       <c r="K25" s="33"/>
       <c r="L25" s="33"/>
       <c r="M25" s="31"/>
       <c r="O25" s="98">
-        <f>SUM(O12:O19)</f>
-        <v>443</v>
-      </c>
-      <c r="P25" s="113"/>
+        <f>SUM(M12:M17)</f>
+        <v>543.5</v>
+      </c>
+      <c r="P25" s="112"/>
     </row>
     <row r="26" spans="2:20">
-      <c r="B26" s="114"/>
+      <c r="B26" s="113"/>
       <c r="C26" s="40"/>
       <c r="D26" s="43"/>
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="50"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="167"/>
       <c r="J26" s="50"/>
       <c r="K26" s="33"/>
       <c r="L26" s="33"/>
       <c r="M26" s="31"/>
       <c r="O26" s="98"/>
-      <c r="P26" s="113"/>
+      <c r="P26" s="112"/>
       <c r="R26" s="91" t="b">
         <f>IF(D26="lt.",C26*J26,IF(D26="gm.",C26/1000*J26,IF(D26="pkt.",C26*J26,IF(D26="kg.",C26*J26,IF(D26="ml.",C26/1000*RJ1510)))))</f>
         <v>0</v>
@@ -2424,20 +2906,20 @@
       </c>
     </row>
     <row r="27" spans="2:20">
-      <c r="B27" s="114"/>
+      <c r="B27" s="113"/>
       <c r="C27" s="40"/>
       <c r="D27" s="71"/>
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="G27" s="47"/>
-      <c r="H27" s="116"/>
+      <c r="H27" s="115"/>
       <c r="I27" s="52"/>
       <c r="J27" s="52"/>
       <c r="K27" s="33"/>
       <c r="L27" s="33"/>
       <c r="M27" s="31"/>
       <c r="O27" s="98"/>
-      <c r="P27" s="113"/>
+      <c r="P27" s="112"/>
       <c r="R27" s="91" t="b">
         <f>IF(D27="lt.",C27*J27,IF(D27="gm.",C27/1000*J27,IF(D27="pkt.",C27*J27,IF(D27="kg.",C27*J27,IF(D27="ml.",C27/1000*RJ1511)))))</f>
         <v>0</v>
@@ -2448,17 +2930,15 @@
       </c>
     </row>
     <row r="28" spans="2:20">
-      <c r="B28" s="114"/>
-      <c r="C28" s="119"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="71"/>
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="47"/>
-      <c r="H28" s="120" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="117"/>
       <c r="K28" s="33"/>
       <c r="L28" s="33"/>
       <c r="M28" s="31"/>
@@ -2469,12 +2949,12 @@
       </c>
     </row>
     <row r="29" spans="2:20">
-      <c r="B29" s="121"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="122">
-        <v>8</v>
+      <c r="D29" s="121">
+        <v>6</v>
       </c>
       <c r="E29" s="101"/>
       <c r="F29" s="101" t="s">
@@ -2482,7 +2962,7 @@
       </c>
       <c r="G29" s="101"/>
       <c r="H29" s="101">
-        <v>443</v>
+        <v>625</v>
       </c>
       <c r="I29" s="88"/>
       <c r="J29" s="101"/>
@@ -2490,18 +2970,12 @@
         <v>18</v>
       </c>
       <c r="L29" s="101"/>
-      <c r="M29" s="123">
+      <c r="M29" s="122">
         <f>SUM(M12:M28)</f>
-        <v>404</v>
+        <v>543.5</v>
       </c>
       <c r="O29" s="98"/>
-      <c r="P29" s="124" t="s">
-        <v>36</v>
-      </c>
-      <c r="R29" s="91" t="e">
-        <f>SUM(R12:R27)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="P29" s="123"/>
       <c r="T29" s="91" t="e">
         <f>SUM(T12:T28)</f>
         <v>#REF!</v>
@@ -2521,7 +2995,7 @@
         <v>32</v>
       </c>
       <c r="L30" s="33"/>
-      <c r="M30" s="125">
+      <c r="M30" s="124">
         <v>0</v>
       </c>
     </row>
@@ -2534,9 +3008,9 @@
         <v>15</v>
       </c>
       <c r="G31" s="33"/>
-      <c r="H31" s="126">
+      <c r="H31" s="125">
         <f>H29-M34</f>
-        <v>39</v>
+        <v>81.5</v>
       </c>
       <c r="I31" s="33"/>
       <c r="J31" s="33"/>
@@ -2544,14 +3018,12 @@
         <v>32</v>
       </c>
       <c r="L31" s="33"/>
-      <c r="M31" s="125">
+      <c r="M31" s="124">
         <v>0</v>
       </c>
-      <c r="O31" s="127"/>
+      <c r="O31" s="126"/>
       <c r="P31" s="98"/>
-      <c r="Q31" s="190" t="s">
-        <v>37</v>
-      </c>
+      <c r="Q31" s="190"/>
       <c r="R31" s="190"/>
       <c r="S31" s="91" t="e">
         <f>T29-R29</f>
@@ -2565,7 +3037,7 @@
       <c r="E32" s="33"/>
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>
-      <c r="H32" s="128" t="s">
+      <c r="H32" s="127" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="33"/>
@@ -2574,7 +3046,7 @@
         <v>19</v>
       </c>
       <c r="L32" s="33"/>
-      <c r="M32" s="125"/>
+      <c r="M32" s="124"/>
     </row>
     <row r="33" spans="1:19">
       <c r="B33" s="93"/>
@@ -2582,14 +3054,14 @@
         <v>16</v>
       </c>
       <c r="D33" s="33"/>
-      <c r="E33" s="129">
+      <c r="E33" s="128">
         <v>0</v>
       </c>
-      <c r="F33" s="129"/>
+      <c r="F33" s="128"/>
       <c r="G33" s="33"/>
-      <c r="H33" s="130">
+      <c r="H33" s="129">
         <f>ROUND(M34,)</f>
-        <v>404</v>
+        <v>544</v>
       </c>
       <c r="I33" s="33"/>
       <c r="J33" s="33"/>
@@ -2597,37 +3069,37 @@
         <v>20</v>
       </c>
       <c r="L33" s="33"/>
-      <c r="M33" s="125"/>
-      <c r="P33" s="127"/>
+      <c r="M33" s="124"/>
+      <c r="P33" s="126"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="B34" s="131"/>
-      <c r="C34" s="132" t="s">
+      <c r="B34" s="130"/>
+      <c r="C34" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="132"/>
-      <c r="E34" s="133">
+      <c r="D34" s="131"/>
+      <c r="E34" s="132">
         <f>ROUND(H33,)</f>
-        <v>404</v>
-      </c>
-      <c r="F34" s="133"/>
-      <c r="G34" s="134"/>
-      <c r="H34" s="134"/>
-      <c r="I34" s="134"/>
-      <c r="J34" s="134"/>
-      <c r="K34" s="132" t="s">
+        <v>544</v>
+      </c>
+      <c r="F34" s="132"/>
+      <c r="G34" s="133"/>
+      <c r="H34" s="133"/>
+      <c r="I34" s="133"/>
+      <c r="J34" s="133"/>
+      <c r="K34" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="L34" s="134"/>
-      <c r="M34" s="135">
+      <c r="L34" s="133"/>
+      <c r="M34" s="134">
         <f>SUM(M29-M32)</f>
-        <v>404</v>
+        <v>543.5</v>
       </c>
       <c r="S34" s="98"/>
     </row>
     <row r="35" spans="1:19">
       <c r="B35" s="186" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="187"/>
       <c r="D35" s="187"/>
@@ -2635,18 +3107,18 @@
       <c r="F35" s="187"/>
       <c r="G35" s="187"/>
       <c r="H35" s="187"/>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="136"/>
-      <c r="M35" s="137"/>
+      <c r="I35" s="135"/>
+      <c r="J35" s="135"/>
+      <c r="K35" s="135"/>
+      <c r="L35" s="135"/>
+      <c r="M35" s="136"/>
     </row>
     <row r="36" spans="1:19">
       <c r="B36" s="176"/>
       <c r="C36" s="171"/>
       <c r="D36" s="171"/>
       <c r="E36" s="177"/>
-      <c r="F36" s="138"/>
+      <c r="F36" s="137"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2665,11 +3137,11 @@
       <c r="C37" s="174"/>
       <c r="D37" s="174"/>
       <c r="E37" s="179"/>
-      <c r="F37" s="139"/>
-      <c r="G37" s="140"/>
-      <c r="H37" s="140"/>
-      <c r="I37" s="140"/>
-      <c r="J37" s="140"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="139"/>
+      <c r="I37" s="139"/>
+      <c r="J37" s="139"/>
       <c r="K37" s="173"/>
       <c r="L37" s="174"/>
       <c r="M37" s="175"/>
@@ -2710,7 +3182,7 @@
     </row>
     <row r="40" spans="1:19" ht="17.25">
       <c r="A40" s="33"/>
-      <c r="B40" s="141"/>
+      <c r="B40" s="140"/>
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
@@ -2736,7 +3208,7 @@
       <c r="J41" s="95"/>
       <c r="K41" s="33"/>
       <c r="L41" s="33"/>
-      <c r="M41" s="142"/>
+      <c r="M41" s="141"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
       <c r="A42" s="33"/>
@@ -2817,7 +3289,7 @@
     </row>
     <row r="47" spans="1:19" ht="15" customHeight="1">
       <c r="B47" s="36"/>
-      <c r="C47" s="143"/>
+      <c r="C47" s="142"/>
       <c r="D47" s="36"/>
       <c r="E47" s="36"/>
       <c r="F47" s="36"/>
@@ -2839,12 +3311,12 @@
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
-      <c r="I48" s="144"/>
+      <c r="I48" s="143"/>
       <c r="J48" s="36"/>
       <c r="K48" s="95"/>
       <c r="L48" s="36"/>
       <c r="M48" s="36"/>
-      <c r="N48" s="145"/>
+      <c r="N48" s="144"/>
       <c r="O48" s="33"/>
     </row>
     <row r="49" spans="2:15" ht="18" thickBot="1">
@@ -2855,7 +3327,7 @@
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
-      <c r="I49" s="144"/>
+      <c r="I49" s="143"/>
       <c r="J49" s="26"/>
       <c r="K49" s="95"/>
       <c r="L49" s="36"/>
@@ -2870,8 +3342,8 @@
       <c r="E50" s="36"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
-      <c r="H50" s="146" t="s">
-        <v>40</v>
+      <c r="H50" s="145" t="s">
+        <v>37</v>
       </c>
       <c r="I50" s="49">
         <v>27</v>
@@ -2887,7 +3359,7 @@
         <v>50</v>
       </c>
       <c r="N50" s="36"/>
-      <c r="O50" s="147"/>
+      <c r="O50" s="146"/>
     </row>
     <row r="51" spans="2:15">
       <c r="B51" s="36"/>
@@ -2897,7 +3369,7 @@
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I51" s="50">
         <v>165</v>
@@ -2913,7 +3385,7 @@
         <v>280</v>
       </c>
       <c r="N51" s="36"/>
-      <c r="O51" s="147"/>
+      <c r="O51" s="146"/>
     </row>
     <row r="52" spans="2:15">
       <c r="B52" s="36"/>
@@ -2922,8 +3394,8 @@
       <c r="E52" s="195"/>
       <c r="F52" s="195"/>
       <c r="G52" s="36"/>
-      <c r="H52" s="148" t="s">
-        <v>53</v>
+      <c r="H52" s="147" t="s">
+        <v>50</v>
       </c>
       <c r="I52" s="50">
         <v>87</v>
@@ -2939,7 +3411,7 @@
         <v>70</v>
       </c>
       <c r="N52" s="36"/>
-      <c r="O52" s="147"/>
+      <c r="O52" s="146"/>
     </row>
     <row r="53" spans="2:15">
       <c r="B53" s="36"/>
@@ -2949,7 +3421,7 @@
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I53" s="50">
         <v>43</v>
@@ -2970,12 +3442,12 @@
     <row r="54" spans="2:15">
       <c r="B54" s="36"/>
       <c r="C54" s="37"/>
-      <c r="D54" s="149"/>
+      <c r="D54" s="148"/>
       <c r="E54" s="36"/>
       <c r="F54" s="36"/>
       <c r="G54" s="36"/>
       <c r="H54" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I54" s="51">
         <v>35</v>
@@ -3001,7 +3473,7 @@
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I55" s="52">
         <v>35</v>
@@ -3016,7 +3488,7 @@
       <c r="M55" s="31">
         <v>70</v>
       </c>
-      <c r="N55" s="149"/>
+      <c r="N55" s="148"/>
       <c r="O55" s="33"/>
     </row>
     <row r="56" spans="2:15">
@@ -3027,7 +3499,7 @@
       <c r="F56" s="36"/>
       <c r="G56" s="36"/>
       <c r="H56" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I56" s="52">
         <v>76</v>
@@ -3053,7 +3525,7 @@
       <c r="F57" s="33"/>
       <c r="G57" s="32"/>
       <c r="H57" s="37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I57" s="52">
         <v>60</v>
@@ -3079,7 +3551,7 @@
       <c r="F58" s="33"/>
       <c r="G58" s="32"/>
       <c r="H58" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I58" s="50">
         <v>310</v>
@@ -3105,7 +3577,7 @@
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
       <c r="H59" s="37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I59" s="50">
         <v>38</v>
@@ -3131,7 +3603,7 @@
       <c r="F60" s="33"/>
       <c r="G60" s="33"/>
       <c r="H60" s="37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I60" s="50">
         <v>20</v>
@@ -3157,7 +3629,7 @@
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I61" s="50">
         <v>10</v>
@@ -3182,8 +3654,8 @@
       <c r="E62" s="33"/>
       <c r="F62" s="33"/>
       <c r="G62" s="33"/>
-      <c r="H62" s="115" t="s">
-        <v>60</v>
+      <c r="H62" s="114" t="s">
+        <v>57</v>
       </c>
       <c r="I62" s="50">
         <v>37</v>
@@ -3208,8 +3680,8 @@
       <c r="E63" s="33"/>
       <c r="F63" s="33"/>
       <c r="G63" s="33"/>
-      <c r="H63" s="115" t="s">
-        <v>61</v>
+      <c r="H63" s="114" t="s">
+        <v>58</v>
       </c>
       <c r="I63" s="50">
         <v>40</v>
@@ -3234,8 +3706,8 @@
       <c r="E64" s="33"/>
       <c r="F64" s="33"/>
       <c r="G64" s="33"/>
-      <c r="H64" s="116" t="s">
-        <v>45</v>
+      <c r="H64" s="115" t="s">
+        <v>42</v>
       </c>
       <c r="I64" s="50">
         <v>51</v>
@@ -3260,8 +3732,8 @@
       <c r="E65" s="33"/>
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
-      <c r="H65" s="116" t="s">
-        <v>46</v>
+      <c r="H65" s="115" t="s">
+        <v>43</v>
       </c>
       <c r="I65" s="52">
         <v>100</v>
@@ -3286,8 +3758,8 @@
       <c r="E66" s="36"/>
       <c r="F66" s="36"/>
       <c r="G66" s="36"/>
-      <c r="H66" s="116" t="s">
-        <v>57</v>
+      <c r="H66" s="115" t="s">
+        <v>54</v>
       </c>
       <c r="I66" s="52">
         <v>60</v>
@@ -3312,17 +3784,17 @@
       <c r="E67" s="37"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
-      <c r="H67" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="I67" s="118">
+      <c r="H67" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="J67" s="118">
+      <c r="I67" s="117">
         <v>45</v>
       </c>
-      <c r="K67" s="118"/>
-      <c r="L67" s="118">
+      <c r="J67" s="117">
+        <v>45</v>
+      </c>
+      <c r="K67" s="117"/>
+      <c r="L67" s="117">
         <v>45</v>
       </c>
       <c r="M67" s="31">
@@ -3338,17 +3810,17 @@
       <c r="E68" s="37"/>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
-      <c r="H68" s="120" t="s">
-        <v>47</v>
-      </c>
-      <c r="I68" s="118">
+      <c r="H68" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="I68" s="117">
         <v>41</v>
       </c>
-      <c r="J68" s="118">
+      <c r="J68" s="117">
         <v>41</v>
       </c>
-      <c r="K68" s="118"/>
-      <c r="L68" s="118">
+      <c r="K68" s="117"/>
+      <c r="L68" s="117">
         <v>41</v>
       </c>
       <c r="M68" s="31">
@@ -3364,17 +3836,17 @@
       <c r="E69" s="37"/>
       <c r="F69" s="36"/>
       <c r="G69" s="36"/>
-      <c r="H69" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="I69" s="118">
+      <c r="H69" s="119" t="s">
+        <v>55</v>
+      </c>
+      <c r="I69" s="117">
         <v>25</v>
       </c>
-      <c r="J69" s="118">
+      <c r="J69" s="117">
         <v>25</v>
       </c>
-      <c r="K69" s="118"/>
-      <c r="L69" s="118">
+      <c r="K69" s="117"/>
+      <c r="L69" s="117">
         <v>25</v>
       </c>
       <c r="M69" s="31">
@@ -3390,17 +3862,17 @@
       <c r="E70" s="37"/>
       <c r="F70" s="36"/>
       <c r="G70" s="36"/>
-      <c r="H70" s="120" t="s">
-        <v>51</v>
-      </c>
-      <c r="I70" s="118">
+      <c r="H70" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="I70" s="117">
         <v>10</v>
       </c>
-      <c r="J70" s="118">
+      <c r="J70" s="117">
         <v>10</v>
       </c>
-      <c r="K70" s="118"/>
-      <c r="L70" s="118">
+      <c r="K70" s="117"/>
+      <c r="L70" s="117">
         <v>10</v>
       </c>
       <c r="M70" s="31">
@@ -3416,17 +3888,17 @@
       <c r="E71" s="37"/>
       <c r="F71" s="36"/>
       <c r="G71" s="36"/>
-      <c r="H71" s="120" t="s">
-        <v>52</v>
-      </c>
-      <c r="I71" s="118">
+      <c r="H71" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="I71" s="117">
         <v>1200</v>
       </c>
-      <c r="J71" s="118">
+      <c r="J71" s="117">
         <v>1000</v>
       </c>
-      <c r="K71" s="118"/>
-      <c r="L71" s="118">
+      <c r="K71" s="117"/>
+      <c r="L71" s="117">
         <v>1000</v>
       </c>
       <c r="M71" s="31">
@@ -3442,23 +3914,23 @@
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
       <c r="G72" s="36"/>
-      <c r="H72" s="120" t="s">
-        <v>49</v>
-      </c>
-      <c r="I72" s="118">
+      <c r="H72" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="I72" s="117">
         <v>69</v>
       </c>
-      <c r="J72" s="118">
+      <c r="J72" s="117">
         <v>66</v>
       </c>
-      <c r="K72" s="118"/>
-      <c r="L72" s="118">
+      <c r="K72" s="117"/>
+      <c r="L72" s="117">
         <v>66</v>
       </c>
       <c r="M72" s="31">
         <v>66</v>
       </c>
-      <c r="N72" s="151"/>
+      <c r="N72" s="149"/>
       <c r="O72" s="33"/>
     </row>
     <row r="73" spans="2:15">
@@ -3468,23 +3940,23 @@
       <c r="E73" s="36"/>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
-      <c r="H73" s="120" t="s">
-        <v>50</v>
-      </c>
-      <c r="I73" s="118">
+      <c r="H73" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="I73" s="117">
         <v>12</v>
       </c>
-      <c r="J73" s="118">
+      <c r="J73" s="117">
         <v>12</v>
       </c>
-      <c r="K73" s="118"/>
-      <c r="L73" s="118">
+      <c r="K73" s="117"/>
+      <c r="L73" s="117">
         <v>12</v>
       </c>
       <c r="M73" s="31">
         <v>60</v>
       </c>
-      <c r="N73" s="151"/>
+      <c r="N73" s="149"/>
       <c r="O73" s="33"/>
     </row>
     <row r="74" spans="2:15">
@@ -3495,12 +3967,12 @@
       <c r="F74" s="36"/>
       <c r="G74" s="36"/>
       <c r="H74" s="36"/>
-      <c r="I74" s="151"/>
+      <c r="I74" s="149"/>
       <c r="J74" s="36"/>
       <c r="K74" s="36"/>
       <c r="L74" s="36"/>
       <c r="M74" s="36"/>
-      <c r="N74" s="151"/>
+      <c r="N74" s="149"/>
       <c r="O74" s="33"/>
     </row>
     <row r="75" spans="2:15">
@@ -3511,12 +3983,12 @@
       <c r="F75" s="36"/>
       <c r="G75" s="36"/>
       <c r="H75" s="36"/>
-      <c r="I75" s="152"/>
+      <c r="I75" s="150"/>
       <c r="J75" s="36"/>
       <c r="K75" s="36"/>
       <c r="L75" s="36"/>
       <c r="M75" s="36"/>
-      <c r="N75" s="151"/>
+      <c r="N75" s="149"/>
       <c r="O75" s="33"/>
     </row>
     <row r="76" spans="2:15">
@@ -3524,31 +3996,31 @@
       <c r="C76" s="36"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
-      <c r="F76" s="151"/>
-      <c r="G76" s="151"/>
+      <c r="F76" s="149"/>
+      <c r="G76" s="149"/>
       <c r="H76" s="36"/>
-      <c r="I76" s="153"/>
+      <c r="I76" s="151"/>
       <c r="J76" s="36"/>
       <c r="K76" s="36"/>
       <c r="L76" s="36"/>
       <c r="M76" s="36"/>
-      <c r="N76" s="151"/>
+      <c r="N76" s="149"/>
       <c r="O76" s="33"/>
     </row>
     <row r="77" spans="2:15">
       <c r="B77" s="36"/>
       <c r="C77" s="36"/>
-      <c r="D77" s="152"/>
-      <c r="E77" s="152"/>
-      <c r="F77" s="153"/>
-      <c r="G77" s="153"/>
+      <c r="D77" s="150"/>
+      <c r="E77" s="150"/>
+      <c r="F77" s="151"/>
+      <c r="G77" s="151"/>
       <c r="H77" s="36"/>
       <c r="I77" s="36"/>
       <c r="J77" s="36"/>
       <c r="K77" s="36"/>
-      <c r="L77" s="152"/>
+      <c r="L77" s="150"/>
       <c r="M77" s="36"/>
-      <c r="N77" s="154"/>
+      <c r="N77" s="152"/>
       <c r="O77" s="33"/>
     </row>
     <row r="78" spans="2:15">
@@ -3573,7 +4045,7 @@
       <c r="D79" s="189"/>
       <c r="E79" s="189"/>
       <c r="F79" s="189"/>
-      <c r="G79" s="155"/>
+      <c r="G79" s="153"/>
       <c r="H79" s="36"/>
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
@@ -3589,7 +4061,7 @@
       <c r="D80" s="189"/>
       <c r="E80" s="189"/>
       <c r="F80" s="189"/>
-      <c r="G80" s="155"/>
+      <c r="G80" s="153"/>
       <c r="H80" s="36"/>
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>

</xml_diff>